<commit_message>
MASTER: Fix top100 features distances.
</commit_message>
<xml_diff>
--- a/doc/subjective evaluation/Features.xlsx
+++ b/doc/subjective evaluation/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssimoes\Documents\GitRepos\MMIRMusicRecommender\doc\subjective evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97F9FB84-1852-402B-952F-57FDB2D7E307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BD6F7A-891E-406E-A713-04F24E401219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88C593F1-7AF5-430A-A3F2-E7FE0FF13C9B}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88C593F1-7AF5-430A-A3F2-E7FE0FF13C9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>MT0000202045</t>
   </si>
@@ -57,258 +57,6 @@
   </si>
   <si>
     <t>Tiago Ventura</t>
-  </si>
-  <si>
-    <t>1 - MT0000202045.mp3 (0.0000)</t>
-  </si>
-  <si>
-    <t>2 - MT0005129157.mp3 (0.0201)</t>
-  </si>
-  <si>
-    <t>3 - MT0012001409.mp3 (0.0202)</t>
-  </si>
-  <si>
-    <t>4 - MT0011899302.mp3 (0.0254)</t>
-  </si>
-  <si>
-    <t>5 - MT0002233402.mp3 (0.0254)</t>
-  </si>
-  <si>
-    <t>6 - MT0002161109.mp3 (0.0292)</t>
-  </si>
-  <si>
-    <t>7 - MT0009217411.mp3 (0.0297)</t>
-  </si>
-  <si>
-    <t>8 - MT0027002641.mp3 (0.0299)</t>
-  </si>
-  <si>
-    <t>9 - MT0000092267.mp3 (0.0301)</t>
-  </si>
-  <si>
-    <t>10 - MT0004428604.mp3 (0.0301)</t>
-  </si>
-  <si>
-    <t>11 - MT0007043504.mp3 (0.0311)</t>
-  </si>
-  <si>
-    <t>12 - MT0010624346.mp3 (0.0312)</t>
-  </si>
-  <si>
-    <t>13 - MT0003787478.mp3 (0.0319)</t>
-  </si>
-  <si>
-    <t>14 - MT0007799677.mp3 (0.0320)</t>
-  </si>
-  <si>
-    <t>15 - MT0011376343.mp3 (0.0322)</t>
-  </si>
-  <si>
-    <t>16 - MT0005261375.mp3 (0.0325)</t>
-  </si>
-  <si>
-    <t>17 - MT0002634024.mp3 (0.0329)</t>
-  </si>
-  <si>
-    <t>18 - MT0006939177.mp3 (0.0332)</t>
-  </si>
-  <si>
-    <t>19 - MT0005213723.mp3 (0.0334)</t>
-  </si>
-  <si>
-    <t>20 - MT0004942017.mp3 (0.0335)</t>
-  </si>
-  <si>
-    <t>21 - MT0002050671.mp3 (0.0335)</t>
-  </si>
-  <si>
-    <t>1 - MT0000379144.mp3 (0.0000)</t>
-  </si>
-  <si>
-    <t>2 - MT0011957429.mp3 (0.0301)</t>
-  </si>
-  <si>
-    <t>3 - MT0004141823.mp3 (0.0332)</t>
-  </si>
-  <si>
-    <t>4 - MT0008222676.mp3 (0.0352)</t>
-  </si>
-  <si>
-    <t>5 - MT0002222957.mp3 (0.0359)</t>
-  </si>
-  <si>
-    <t>6 - MT0006510599.mp3 (0.0368)</t>
-  </si>
-  <si>
-    <t>7 - MT0005202791.mp3 (0.0375)</t>
-  </si>
-  <si>
-    <t>8 - MT0006164654.mp3 (0.0376)</t>
-  </si>
-  <si>
-    <t>9 - MT0006742179.mp3 (0.0393)</t>
-  </si>
-  <si>
-    <t>10 - MT0004956006.mp3 (0.0400)</t>
-  </si>
-  <si>
-    <t>11 - MT0012124855.mp3 (0.0400)</t>
-  </si>
-  <si>
-    <t>12 - MT0012041920.mp3 (0.0400)</t>
-  </si>
-  <si>
-    <t>13 - MT0029772184.mp3 (0.0404)</t>
-  </si>
-  <si>
-    <t>14 - MT0009041370.mp3 (0.0407)</t>
-  </si>
-  <si>
-    <t>15 - MT0007379559.mp3 (0.0408)</t>
-  </si>
-  <si>
-    <t>16 - MT0005515169.mp3 (0.0409)</t>
-  </si>
-  <si>
-    <t>17 - MT0006540794.mp3 (0.0419)</t>
-  </si>
-  <si>
-    <t>18 - MT0007659703.mp3 (0.0423)</t>
-  </si>
-  <si>
-    <t>19 - MT0003546058.mp3 (0.0424)</t>
-  </si>
-  <si>
-    <t>20 - MT0005606947.mp3 (0.0426)</t>
-  </si>
-  <si>
-    <t>21 - MT0010465830.mp3 (0.0430)</t>
-  </si>
-  <si>
-    <t>1 - MT0000414517.mp3 (0.0000)</t>
-  </si>
-  <si>
-    <t>2 - MT0004274911.mp3 (0.0578)</t>
-  </si>
-  <si>
-    <t>3 - MT0002634024.mp3 (0.0593)</t>
-  </si>
-  <si>
-    <t>4 - MT0009521580.mp3 (0.0607)</t>
-  </si>
-  <si>
-    <t>5 - MT0003900455.mp3 (0.0619)</t>
-  </si>
-  <si>
-    <t>6 - MT0003949060.mp3 (0.0627)</t>
-  </si>
-  <si>
-    <t>7 - MT0008401073.mp3 (0.0631)</t>
-  </si>
-  <si>
-    <t>8 - MT0000901959.mp3 (0.0644)</t>
-  </si>
-  <si>
-    <t>9 - MT0009897495.mp3 (0.0645)</t>
-  </si>
-  <si>
-    <t>10 - MT0005469880.mp3 (0.0646)</t>
-  </si>
-  <si>
-    <t>11 - MT0002415184.mp3 (0.0647)</t>
-  </si>
-  <si>
-    <t>12 - MT0000040632.mp3 (0.0654)</t>
-  </si>
-  <si>
-    <t>13 - MT0009991160.mp3 (0.0657)</t>
-  </si>
-  <si>
-    <t>14 - MT0000218346.mp3 (0.0669)</t>
-  </si>
-  <si>
-    <t>15 - MT0008972801.mp3 (0.0670)</t>
-  </si>
-  <si>
-    <t>16 - MT0000255724.mp3 (0.0671)</t>
-  </si>
-  <si>
-    <t>17 - MT0001942272.mp3 (0.0674)</t>
-  </si>
-  <si>
-    <t>18 - MT0000636335.mp3 (0.0679)</t>
-  </si>
-  <si>
-    <t>19 - MT0001583214.mp3 (0.0688)</t>
-  </si>
-  <si>
-    <t>20 - MT0032181833.mp3 (0.0689)</t>
-  </si>
-  <si>
-    <t>21 - MT0006410285.mp3 (0.0690)</t>
-  </si>
-  <si>
-    <t>1 - MT0000956340.mp3 (0.0000)</t>
-  </si>
-  <si>
-    <t>2 - MT0006096934.mp3 (0.0239)</t>
-  </si>
-  <si>
-    <t>3 - MT0003603772.mp3 (0.0247)</t>
-  </si>
-  <si>
-    <t>4 - MT0040033011.mp3 (0.0258)</t>
-  </si>
-  <si>
-    <t>5 - MT0005625762.mp3 (0.0263)</t>
-  </si>
-  <si>
-    <t>6 - MT0003787478.mp3 (0.0268)</t>
-  </si>
-  <si>
-    <t>7 - MT0011145388.mp3 (0.0292)</t>
-  </si>
-  <si>
-    <t>8 - MT0033177286.mp3 (0.0296)</t>
-  </si>
-  <si>
-    <t>9 - MT0006640142.mp3 (0.0307)</t>
-  </si>
-  <si>
-    <t>10 - MT0013389935.mp3 (0.0314)</t>
-  </si>
-  <si>
-    <t>11 - MT0008511909.mp3 (0.0320)</t>
-  </si>
-  <si>
-    <t>12 - MT0003213835.mp3 (0.0323)</t>
-  </si>
-  <si>
-    <t>13 - MT0005331755.mp3 (0.0324)</t>
-  </si>
-  <si>
-    <t>14 - MT0004958762.mp3 (0.0332)</t>
-  </si>
-  <si>
-    <t>15 - MT0005409948.mp3 (0.0336)</t>
-  </si>
-  <si>
-    <t>16 - MT0004867185.mp3 (0.0339)</t>
-  </si>
-  <si>
-    <t>17 - MT0005265641.mp3 (0.0342)</t>
-  </si>
-  <si>
-    <t>18 - MT0009213083.mp3 (0.0345)</t>
-  </si>
-  <si>
-    <t>19 - MT0004807446.mp3 (0.0355)</t>
-  </si>
-  <si>
-    <t>20 - MT0004537445.mp3 (0.0360)</t>
-  </si>
-  <si>
-    <t>21 - MT0001217651.mp3 (0.0361)</t>
   </si>
 </sst>
 </file>
@@ -474,16 +222,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -807,55 +555,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E1B9E6-B0FF-4E99-81BB-013559980CEC}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -894,8 +642,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
@@ -911,8 +659,8 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
@@ -928,8 +676,8 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
@@ -945,8 +693,8 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
@@ -962,8 +710,8 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
@@ -979,8 +727,8 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
@@ -996,8 +744,8 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
@@ -1013,8 +761,8 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
@@ -1030,8 +778,8 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="1"/>
@@ -1047,8 +795,8 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="1"/>
@@ -1064,8 +812,8 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="1"/>
@@ -1081,8 +829,8 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="1"/>
@@ -1098,8 +846,8 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="1"/>
@@ -1115,8 +863,8 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" s="1"/>
@@ -1132,8 +880,8 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="1"/>
@@ -1149,8 +897,8 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="1"/>
@@ -1166,8 +914,8 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" s="1"/>
@@ -1183,8 +931,8 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" s="1"/>
@@ -1200,8 +948,8 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21" s="1"/>
@@ -1217,8 +965,8 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="1"/>
@@ -1233,300 +981,6 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" t="s">
-        <v>50</v>
-      </c>
-      <c r="J25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" t="s">
-        <v>52</v>
-      </c>
-      <c r="J27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" t="s">
-        <v>53</v>
-      </c>
-      <c r="J28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-      <c r="G31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-      <c r="G33" t="s">
-        <v>58</v>
-      </c>
-      <c r="J33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" t="s">
-        <v>59</v>
-      </c>
-      <c r="J34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" t="s">
-        <v>60</v>
-      </c>
-      <c r="J35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" t="s">
-        <v>61</v>
-      </c>
-      <c r="J36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" t="s">
-        <v>41</v>
-      </c>
-      <c r="G37" t="s">
-        <v>62</v>
-      </c>
-      <c r="J37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" t="s">
-        <v>63</v>
-      </c>
-      <c r="J38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" t="s">
-        <v>64</v>
-      </c>
-      <c r="J39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" t="s">
-        <v>65</v>
-      </c>
-      <c r="J40" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" t="s">
-        <v>66</v>
-      </c>
-      <c r="J41" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" t="s">
-        <v>67</v>
-      </c>
-      <c r="J42" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" t="s">
-        <v>47</v>
-      </c>
-      <c r="G43" t="s">
-        <v>68</v>
-      </c>
-      <c r="J43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G44" t="s">
-        <v>69</v>
-      </c>
-      <c r="J44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" t="s">
-        <v>70</v>
-      </c>
-      <c r="J45" t="s">
-        <v>91</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>